<commit_message>
updated tests for kiz and wg; bug in favorability_check corrected; Entgeltpunkte now imputed
Former-commit-id: cac9008a854b2bf7b9fc4c39f059b7bb512a4691
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_kiz.xlsx
+++ b/tests/test_data/test_dfs_kiz.xlsx
@@ -97,9 +97,6 @@
     <t>m_alg2</t>
   </si>
   <si>
-    <t>wohngeld_init</t>
-  </si>
-  <si>
     <t>fehlbedarf_alg2</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t>wgkiz_vorrang</t>
+  </si>
+  <si>
+    <t>wohngeld_basis_hh</t>
   </si>
 </sst>
 </file>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM15" sqref="AM15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +549,7 @@
     <col min="30" max="30" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -557,7 +557,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>6</v>
@@ -596,13 +596,13 @@
         <v>13</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S1" s="12" t="s">
         <v>10</v>
@@ -644,25 +644,25 @@
         <v>24</v>
       </c>
       <c r="AH1" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AI1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="12" t="s">
+      <c r="AK1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="12" t="s">
+      <c r="AL1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="12" t="s">
+      <c r="AM1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="12" t="s">
+      <c r="AN1" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="AN1" s="12" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
@@ -900,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="AG3" s="8">
-        <f t="shared" ref="AG3:AG16" si="10">AE3*170*M3-AF3</f>
+        <f t="shared" ref="AG3:AG13" si="10">AE3*170*M3-AF3</f>
         <v>170</v>
       </c>
       <c r="AH3" s="28">

</xml_diff>

<commit_message>
kiz test correction #2
Former-commit-id: 00edfaebd8cacd4d461177c377069652b8c33232
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_kiz.xlsx
+++ b/tests/test_data/test_dfs_kiz.xlsx
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,10 +740,10 @@
       </c>
       <c r="W2" s="1">
         <f>IF(OR($AN2=TRUE,$AO2=TRUE),$AH2,0)</f>
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="X2" s="1">
-        <f>IF(AND($AM2=FALSE,$AN2=FALSE,$AO2=FALSE),$S2,0)</f>
+        <f>IF(AND($AM2=FALSE,$AN2=FALSE,$AO2=FALSE),$AI2,0)</f>
         <v>0</v>
       </c>
       <c r="Y2" s="1">
@@ -776,8 +776,8 @@
         <v>0</v>
       </c>
       <c r="AH2" s="8">
-        <f>AF2*170*N2-AG2</f>
-        <v>170</v>
+        <f>AF2*140*N2-AG2</f>
+        <v>140</v>
       </c>
       <c r="AI2" s="28">
         <f>MAX(R2-S2,0)</f>
@@ -789,7 +789,7 @@
       </c>
       <c r="AK2" s="28">
         <f>MAX(R2-S2-AH2,0)</f>
-        <v>295</v>
+        <v>325</v>
       </c>
       <c r="AL2" s="28">
         <f>MAX(R2-S2-Q2-AH2,0)</f>
@@ -876,10 +876,10 @@
       </c>
       <c r="W3" s="11">
         <f t="shared" ref="W3:W16" si="1">IF(OR($AN3=TRUE,$AO3=TRUE),$AH3,0)</f>
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="X3" s="1">
-        <f t="shared" ref="X3:X16" si="2">IF(AND($AM3=FALSE,$AN3=FALSE,$AO3=FALSE),$S3,0)</f>
+        <f t="shared" ref="X3:X16" si="2">IF(AND($AM3=FALSE,$AN3=FALSE,$AO3=FALSE),$AI3,0)</f>
         <v>0</v>
       </c>
       <c r="Y3" s="1">
@@ -912,35 +912,35 @@
         <v>0</v>
       </c>
       <c r="AH3" s="8">
-        <f t="shared" ref="AH3:AH13" si="10">AF3*170*N3-AG3</f>
-        <v>170</v>
+        <f>AF3*140*N3-AG3</f>
+        <v>140</v>
       </c>
       <c r="AI3" s="28">
-        <f t="shared" ref="AI3:AI16" si="11">MAX(R3-S3,0)</f>
+        <f t="shared" ref="AI3:AI16" si="10">MAX(R3-S3,0)</f>
         <v>465</v>
       </c>
       <c r="AJ3" s="28">
-        <f t="shared" ref="AJ3:AJ16" si="12">MAX(R3-S3-Q3,0)</f>
+        <f t="shared" ref="AJ3:AJ16" si="11">MAX(R3-S3-Q3,0)</f>
         <v>115</v>
       </c>
       <c r="AK3" s="28">
-        <f t="shared" ref="AK3:AK16" si="13">MAX(R3-S3-AH3,0)</f>
-        <v>295</v>
+        <f t="shared" ref="AK3:AK16" si="12">MAX(R3-S3-AH3,0)</f>
+        <v>325</v>
       </c>
       <c r="AL3" s="28">
-        <f t="shared" ref="AL3:AL16" si="14">MAX(R3-S3-Q3-AH3,0)</f>
+        <f t="shared" ref="AL3:AL16" si="13">MAX(R3-S3-Q3-AH3,0)</f>
         <v>0</v>
       </c>
       <c r="AM3" t="b">
-        <f t="shared" ref="AM3:AM16" si="15">AND(AJ3=0,AI3&gt;0)</f>
+        <f t="shared" ref="AM3:AM16" si="14">AND(AJ3=0,AI3&gt;0)</f>
         <v>0</v>
       </c>
       <c r="AN3" t="b">
-        <f t="shared" ref="AN3:AN16" si="16">AND(AK3=0,AI3&gt;0)</f>
+        <f t="shared" ref="AN3:AN16" si="15">AND(AK3=0,AI3&gt;0)</f>
         <v>0</v>
       </c>
       <c r="AO3" t="b">
-        <f t="shared" ref="AO3:AO16" si="17">AND(AL3=0,AI3&gt;0)</f>
+        <f t="shared" ref="AO3:AO16" si="16">AND(AL3=0,AI3&gt;0)</f>
         <v>1</v>
       </c>
     </row>
@@ -1012,7 +1012,7 @@
       </c>
       <c r="W4" s="11">
         <f t="shared" si="1"/>
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="X4" s="1">
         <f t="shared" si="2"/>
@@ -1048,35 +1048,35 @@
         <v>0</v>
       </c>
       <c r="AH4" s="8">
+        <f>AF4*140*N4-AG4</f>
+        <v>140</v>
+      </c>
+      <c r="AI4" s="28">
         <f t="shared" si="10"/>
-        <v>170</v>
-      </c>
-      <c r="AI4" s="28">
+        <v>465</v>
+      </c>
+      <c r="AJ4" s="28">
         <f t="shared" si="11"/>
-        <v>465</v>
-      </c>
-      <c r="AJ4" s="28">
+        <v>115</v>
+      </c>
+      <c r="AK4" s="28">
         <f t="shared" si="12"/>
-        <v>115</v>
-      </c>
-      <c r="AK4" s="28">
+        <v>325</v>
+      </c>
+      <c r="AL4" s="28">
         <f t="shared" si="13"/>
-        <v>295</v>
-      </c>
-      <c r="AL4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AM4" t="b">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AM4" t="b">
+      <c r="AN4" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AN4" t="b">
+      <c r="AO4" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO4" t="b">
-        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
@@ -1150,9 +1150,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X5" s="18">
+      <c r="X5" s="1">
         <f t="shared" si="2"/>
-        <v>700</v>
+        <v>470</v>
       </c>
       <c r="Y5" s="18">
         <f t="shared" si="3"/>
@@ -1176,35 +1176,35 @@
         <v>0</v>
       </c>
       <c r="AH5" s="9">
+        <f>AF5*140*N5-AG5</f>
+        <v>0</v>
+      </c>
+      <c r="AI5" s="29">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AI5" s="29">
+        <v>470</v>
+      </c>
+      <c r="AJ5" s="29">
         <f t="shared" si="11"/>
+        <v>70</v>
+      </c>
+      <c r="AK5" s="29">
+        <f t="shared" si="12"/>
         <v>470</v>
       </c>
-      <c r="AJ5" s="29">
-        <f t="shared" si="12"/>
+      <c r="AL5" s="28">
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
-      <c r="AK5" s="29">
-        <f t="shared" si="13"/>
-        <v>470</v>
-      </c>
-      <c r="AL5" s="28">
+      <c r="AM5" t="b">
         <f t="shared" si="14"/>
-        <v>70</v>
-      </c>
-      <c r="AM5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN5" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AN5" t="b">
+      <c r="AO5" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO5" t="b">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -1278,9 +1278,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X6" s="19">
+      <c r="X6" s="1">
         <f t="shared" si="2"/>
-        <v>700</v>
+        <v>470</v>
       </c>
       <c r="Y6" s="19">
         <f t="shared" si="3"/>
@@ -1303,35 +1303,35 @@
         <v>0</v>
       </c>
       <c r="AH6" s="17">
+        <f>AF6*140*N6-AG6</f>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="30">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AI6" s="30">
+        <v>470</v>
+      </c>
+      <c r="AJ6" s="30">
         <f t="shared" si="11"/>
+        <v>70</v>
+      </c>
+      <c r="AK6" s="30">
+        <f t="shared" si="12"/>
         <v>470</v>
       </c>
-      <c r="AJ6" s="30">
-        <f t="shared" si="12"/>
+      <c r="AL6" s="28">
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
-      <c r="AK6" s="30">
-        <f t="shared" si="13"/>
-        <v>470</v>
-      </c>
-      <c r="AL6" s="28">
+      <c r="AM6" t="b">
         <f t="shared" si="14"/>
-        <v>70</v>
-      </c>
-      <c r="AM6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN6" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AN6" t="b">
+      <c r="AO6" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO6" t="b">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -1403,9 +1403,9 @@
       </c>
       <c r="W7" s="20">
         <f t="shared" si="1"/>
-        <v>170</v>
-      </c>
-      <c r="X7" s="18">
+        <v>140</v>
+      </c>
+      <c r="X7" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1440,35 +1440,35 @@
         <v>0</v>
       </c>
       <c r="AH7" s="9">
+        <f>AF7*140*N7-AG7</f>
+        <v>140</v>
+      </c>
+      <c r="AI7" s="29">
         <f t="shared" si="10"/>
-        <v>170</v>
-      </c>
-      <c r="AI7" s="29">
+        <v>628.63999999999987</v>
+      </c>
+      <c r="AJ7" s="29">
         <f t="shared" si="11"/>
-        <v>628.63999999999987</v>
-      </c>
-      <c r="AJ7" s="29">
+        <v>128.63999999999987</v>
+      </c>
+      <c r="AK7" s="29">
         <f t="shared" si="12"/>
-        <v>128.63999999999987</v>
-      </c>
-      <c r="AK7" s="29">
+        <v>488.63999999999987</v>
+      </c>
+      <c r="AL7" s="28">
         <f t="shared" si="13"/>
-        <v>458.63999999999987</v>
-      </c>
-      <c r="AL7" s="28">
+        <v>0</v>
+      </c>
+      <c r="AM7" t="b">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AM7" t="b">
+      <c r="AN7" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AN7" t="b">
+      <c r="AO7" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO7" t="b">
-        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
@@ -1540,9 +1540,9 @@
       </c>
       <c r="W8" s="21">
         <f t="shared" si="1"/>
-        <v>170</v>
-      </c>
-      <c r="X8" s="19">
+        <v>140</v>
+      </c>
+      <c r="X8" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1576,35 +1576,35 @@
         <v>0</v>
       </c>
       <c r="AH8" s="8">
+        <f>AF8*140*N8-AG8</f>
+        <v>140</v>
+      </c>
+      <c r="AI8" s="31">
         <f t="shared" si="10"/>
-        <v>170</v>
-      </c>
-      <c r="AI8" s="31">
+        <v>628.63999999999987</v>
+      </c>
+      <c r="AJ8" s="31">
         <f t="shared" si="11"/>
-        <v>628.63999999999987</v>
-      </c>
-      <c r="AJ8" s="31">
+        <v>128.63999999999987</v>
+      </c>
+      <c r="AK8" s="31">
         <f t="shared" si="12"/>
-        <v>128.63999999999987</v>
-      </c>
-      <c r="AK8" s="31">
+        <v>488.63999999999987</v>
+      </c>
+      <c r="AL8" s="28">
         <f t="shared" si="13"/>
-        <v>458.63999999999987</v>
-      </c>
-      <c r="AL8" s="28">
+        <v>0</v>
+      </c>
+      <c r="AM8" t="b">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AM8" t="b">
+      <c r="AN8" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AN8" t="b">
+      <c r="AO8" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO8" t="b">
-        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
@@ -1679,9 +1679,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X9" s="18">
+      <c r="X9" s="1">
         <f t="shared" si="2"/>
-        <v>462</v>
+        <v>1819</v>
       </c>
       <c r="Y9" s="18">
         <f t="shared" si="3"/>
@@ -1702,7 +1702,7 @@
         <v>1223.5639999999999</v>
       </c>
       <c r="AE9" s="14">
-        <f t="shared" ref="AE9:AE13" si="18">AD9+140*N9</f>
+        <f t="shared" ref="AE9:AE13" si="17">AD9+140*N9</f>
         <v>1643.5639999999999</v>
       </c>
       <c r="AF9" s="2" t="b">
@@ -1714,35 +1714,35 @@
         <v>140</v>
       </c>
       <c r="AH9" s="9">
-        <f>AF9*170*N9-AG9</f>
-        <v>370</v>
+        <f>AF9*140*N9-AG9</f>
+        <v>280</v>
       </c>
       <c r="AI9" s="32">
+        <f t="shared" si="10"/>
+        <v>1819</v>
+      </c>
+      <c r="AJ9" s="29">
         <f t="shared" si="11"/>
-        <v>1819</v>
-      </c>
-      <c r="AJ9" s="29">
+        <v>1169</v>
+      </c>
+      <c r="AK9" s="32">
         <f t="shared" si="12"/>
-        <v>1169</v>
-      </c>
-      <c r="AK9" s="32">
+        <v>1539</v>
+      </c>
+      <c r="AL9" s="28">
         <f t="shared" si="13"/>
-        <v>1449</v>
-      </c>
-      <c r="AL9" s="28">
+        <v>889</v>
+      </c>
+      <c r="AM9" t="b">
         <f t="shared" si="14"/>
-        <v>799</v>
-      </c>
-      <c r="AM9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN9" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AN9" t="b">
+      <c r="AO9" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO9" t="b">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
         <v>462</v>
       </c>
       <c r="T10" s="3">
-        <f t="shared" ref="T10:T13" si="19">3*154</f>
+        <f t="shared" ref="T10:T13" si="18">3*154</f>
         <v>462</v>
       </c>
       <c r="U10" s="3"/>
@@ -1817,20 +1817,20 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X10" s="19">
+      <c r="X10" s="1">
         <f t="shared" si="2"/>
-        <v>462</v>
+        <v>1819</v>
       </c>
       <c r="Y10" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA10" s="3">
-        <f t="shared" ref="AA10:AA13" si="20">345*0.9*2</f>
+        <f t="shared" ref="AA10:AA13" si="19">345*0.9*2</f>
         <v>621</v>
       </c>
       <c r="AB10" s="8">
-        <f t="shared" ref="AB10:AB13" si="21">0.6212*(I10+J10)</f>
+        <f t="shared" ref="AB10:AB13" si="20">0.6212*(I10+J10)</f>
         <v>602.56399999999996</v>
       </c>
       <c r="AC10" s="8"/>
@@ -1839,7 +1839,7 @@
         <v>1223.5639999999999</v>
       </c>
       <c r="AE10" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>1643.5639999999999</v>
       </c>
       <c r="AF10" s="4" t="b">
@@ -1851,35 +1851,35 @@
         <v>140</v>
       </c>
       <c r="AH10" s="8">
+        <f>AF10*140*N10-AG10</f>
+        <v>280</v>
+      </c>
+      <c r="AI10" s="33">
         <f t="shared" si="10"/>
-        <v>370</v>
-      </c>
-      <c r="AI10" s="33">
+        <v>1819</v>
+      </c>
+      <c r="AJ10" s="31">
         <f t="shared" si="11"/>
-        <v>1819</v>
-      </c>
-      <c r="AJ10" s="31">
+        <v>1169</v>
+      </c>
+      <c r="AK10" s="33">
         <f t="shared" si="12"/>
-        <v>1169</v>
-      </c>
-      <c r="AK10" s="33">
+        <v>1539</v>
+      </c>
+      <c r="AL10" s="28">
         <f t="shared" si="13"/>
-        <v>1449</v>
-      </c>
-      <c r="AL10" s="28">
+        <v>889</v>
+      </c>
+      <c r="AM10" t="b">
         <f t="shared" si="14"/>
-        <v>799</v>
-      </c>
-      <c r="AM10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN10" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AN10" t="b">
+      <c r="AO10" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO10" t="b">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -1943,7 +1943,7 @@
         <v>462</v>
       </c>
       <c r="T11" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>462</v>
       </c>
       <c r="U11" s="3"/>
@@ -1954,20 +1954,20 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X11" s="19">
+      <c r="X11" s="1">
         <f t="shared" si="2"/>
-        <v>462</v>
+        <v>1819</v>
       </c>
       <c r="Y11" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA11" s="3">
+        <f t="shared" si="19"/>
+        <v>621</v>
+      </c>
+      <c r="AB11" s="8">
         <f t="shared" si="20"/>
-        <v>621</v>
-      </c>
-      <c r="AB11" s="8">
-        <f t="shared" si="21"/>
         <v>602.56399999999996</v>
       </c>
       <c r="AC11" s="8"/>
@@ -1976,7 +1976,7 @@
         <v>1223.5639999999999</v>
       </c>
       <c r="AE11" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>1643.5639999999999</v>
       </c>
       <c r="AF11" t="b">
@@ -1988,35 +1988,35 @@
         <v>140</v>
       </c>
       <c r="AH11" s="8">
+        <f>AF11*140*N11-AG11</f>
+        <v>280</v>
+      </c>
+      <c r="AI11" s="28">
         <f t="shared" si="10"/>
-        <v>370</v>
-      </c>
-      <c r="AI11" s="28">
+        <v>1819</v>
+      </c>
+      <c r="AJ11" s="31">
         <f t="shared" si="11"/>
-        <v>1819</v>
-      </c>
-      <c r="AJ11" s="31">
+        <v>1169</v>
+      </c>
+      <c r="AK11" s="28">
         <f t="shared" si="12"/>
-        <v>1169</v>
-      </c>
-      <c r="AK11" s="28">
+        <v>1539</v>
+      </c>
+      <c r="AL11" s="28">
         <f t="shared" si="13"/>
-        <v>1449</v>
-      </c>
-      <c r="AL11" s="28">
+        <v>889</v>
+      </c>
+      <c r="AM11" t="b">
         <f t="shared" si="14"/>
-        <v>799</v>
-      </c>
-      <c r="AM11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN11" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AN11" t="b">
+      <c r="AO11" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO11" t="b">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -2080,7 +2080,7 @@
         <v>462</v>
       </c>
       <c r="T12" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>462</v>
       </c>
       <c r="U12" s="3"/>
@@ -2091,9 +2091,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X12" s="19">
+      <c r="X12" s="1">
         <f t="shared" si="2"/>
-        <v>462</v>
+        <v>1819</v>
       </c>
       <c r="Y12" s="19">
         <f t="shared" si="3"/>
@@ -2101,11 +2101,11 @@
       </c>
       <c r="Z12" s="22"/>
       <c r="AA12" s="3">
+        <f t="shared" si="19"/>
+        <v>621</v>
+      </c>
+      <c r="AB12" s="8">
         <f t="shared" si="20"/>
-        <v>621</v>
-      </c>
-      <c r="AB12" s="8">
-        <f t="shared" si="21"/>
         <v>602.56399999999996</v>
       </c>
       <c r="AC12" s="8"/>
@@ -2114,7 +2114,7 @@
         <v>1223.5639999999999</v>
       </c>
       <c r="AE12" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>1643.5639999999999</v>
       </c>
       <c r="AF12" t="b">
@@ -2126,35 +2126,35 @@
         <v>140</v>
       </c>
       <c r="AH12" s="8">
+        <f>AF12*140*N12-AG12</f>
+        <v>280</v>
+      </c>
+      <c r="AI12" s="28">
         <f t="shared" si="10"/>
-        <v>370</v>
-      </c>
-      <c r="AI12" s="28">
+        <v>1819</v>
+      </c>
+      <c r="AJ12" s="31">
         <f t="shared" si="11"/>
-        <v>1819</v>
-      </c>
-      <c r="AJ12" s="31">
+        <v>1169</v>
+      </c>
+      <c r="AK12" s="28">
         <f t="shared" si="12"/>
-        <v>1169</v>
-      </c>
-      <c r="AK12" s="28">
+        <v>1539</v>
+      </c>
+      <c r="AL12" s="28">
         <f t="shared" si="13"/>
-        <v>1449</v>
-      </c>
-      <c r="AL12" s="28">
+        <v>889</v>
+      </c>
+      <c r="AM12" t="b">
         <f t="shared" si="14"/>
-        <v>799</v>
-      </c>
-      <c r="AM12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AN12" t="b">
+      <c r="AO12" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO12" t="b">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -2218,7 +2218,7 @@
         <v>462</v>
       </c>
       <c r="T13" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>462</v>
       </c>
       <c r="U13" s="3"/>
@@ -2229,9 +2229,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X13" s="19">
+      <c r="X13" s="1">
         <f t="shared" si="2"/>
-        <v>462</v>
+        <v>1819</v>
       </c>
       <c r="Y13" s="19">
         <f t="shared" si="3"/>
@@ -2239,11 +2239,11 @@
       </c>
       <c r="Z13" s="22"/>
       <c r="AA13" s="3">
+        <f t="shared" si="19"/>
+        <v>621</v>
+      </c>
+      <c r="AB13" s="8">
         <f t="shared" si="20"/>
-        <v>621</v>
-      </c>
-      <c r="AB13" s="8">
-        <f t="shared" si="21"/>
         <v>602.56399999999996</v>
       </c>
       <c r="AC13" s="8"/>
@@ -2252,7 +2252,7 @@
         <v>1223.5639999999999</v>
       </c>
       <c r="AE13" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>1643.5639999999999</v>
       </c>
       <c r="AF13" t="b">
@@ -2264,35 +2264,35 @@
         <v>140</v>
       </c>
       <c r="AH13" s="8">
+        <f>AF13*140*N13-AG13</f>
+        <v>280</v>
+      </c>
+      <c r="AI13" s="28">
         <f t="shared" si="10"/>
-        <v>370</v>
-      </c>
-      <c r="AI13" s="28">
+        <v>1819</v>
+      </c>
+      <c r="AJ13" s="31">
         <f t="shared" si="11"/>
-        <v>1819</v>
-      </c>
-      <c r="AJ13" s="31">
+        <v>1169</v>
+      </c>
+      <c r="AK13" s="28">
         <f t="shared" si="12"/>
-        <v>1169</v>
-      </c>
-      <c r="AK13" s="28">
+        <v>1539</v>
+      </c>
+      <c r="AL13" s="28">
         <f t="shared" si="13"/>
-        <v>1449</v>
-      </c>
-      <c r="AL13" s="28">
+        <v>889</v>
+      </c>
+      <c r="AM13" t="b">
         <f t="shared" si="14"/>
-        <v>799</v>
-      </c>
-      <c r="AM13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN13" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AN13" t="b">
+      <c r="AO13" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO13" t="b">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X14" s="18">
+      <c r="X14" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2394,31 +2394,31 @@
         <v>0</v>
       </c>
       <c r="AI14" s="28">
+        <f t="shared" si="10"/>
+        <v>125</v>
+      </c>
+      <c r="AJ14" s="28">
         <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AK14" s="28">
+        <f t="shared" si="12"/>
         <v>125</v>
       </c>
-      <c r="AJ14" s="28">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AK14" s="28">
+      <c r="AL14" s="28">
         <f t="shared" si="13"/>
-        <v>125</v>
-      </c>
-      <c r="AL14" s="28">
+        <v>0</v>
+      </c>
+      <c r="AM14" t="b">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AM14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN14" t="b">
         <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="AN14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO14" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO14" t="b">
-        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="Z15" s="3"/>
       <c r="AA15">
-        <f t="shared" ref="AA15:AA16" si="22">3*291</f>
+        <f t="shared" ref="AA15:AA16" si="21">3*291</f>
         <v>873</v>
       </c>
       <c r="AD15" s="24">
@@ -2516,31 +2516,31 @@
         <v>0</v>
       </c>
       <c r="AI15" s="28">
+        <f t="shared" si="10"/>
+        <v>125</v>
+      </c>
+      <c r="AJ15" s="28">
         <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AK15" s="28">
+        <f t="shared" si="12"/>
         <v>125</v>
       </c>
-      <c r="AJ15" s="28">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AK15" s="28">
+      <c r="AL15" s="28">
         <f t="shared" si="13"/>
-        <v>125</v>
-      </c>
-      <c r="AL15" s="28">
+        <v>0</v>
+      </c>
+      <c r="AM15" t="b">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AM15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN15" t="b">
         <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="AN15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO15" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO15" t="b">
-        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
@@ -2613,7 +2613,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X16" s="19">
+      <c r="X16" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2623,7 +2623,7 @@
       </c>
       <c r="Z16" s="3"/>
       <c r="AA16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>873</v>
       </c>
       <c r="AD16" s="24">
@@ -2638,31 +2638,31 @@
         <v>0</v>
       </c>
       <c r="AI16" s="28">
+        <f t="shared" si="10"/>
+        <v>125</v>
+      </c>
+      <c r="AJ16" s="28">
         <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AK16" s="28">
+        <f t="shared" si="12"/>
         <v>125</v>
       </c>
-      <c r="AJ16" s="28">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AK16" s="28">
+      <c r="AL16" s="28">
         <f t="shared" si="13"/>
-        <v>125</v>
-      </c>
-      <c r="AL16" s="28">
+        <v>0</v>
+      </c>
+      <c r="AM16" t="b">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AM16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN16" t="b">
         <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="AN16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO16" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AO16" t="b">
-        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>